<commit_message>
o excel de output já está melhorzito
</commit_message>
<xml_diff>
--- a/output/Output-Avaliacao-Membro-RH.xlsx
+++ b/output/Output-Avaliacao-Membro-RH.xlsx
@@ -413,14 +413,771 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:A1"/>
+  <dimension ref="A1:E28"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
-  <sheetData/>
+  <sheetData>
+    <row r="1" ht="217.2" customHeight="1">
+      <c r="A1" t="inlineStr">
+        <is>
+          <t>Avaliador</t>
+        </is>
+      </c>
+      <c r="B1" t="inlineStr">
+        <is>
+          <t>Avaliado</t>
+        </is>
+      </c>
+      <c r="C1" t="inlineStr">
+        <is>
+          <t>1. O membro coopera com os seus colegas para alcançar objetivos comuns que tenham sido estabelecidos.</t>
+        </is>
+      </c>
+      <c r="D1" t="inlineStr">
+        <is>
+          <t>2. O membro assume, em regra, objetivos ambiciosos e exigentes, embora realistas, para si e para os seus colegas.</t>
+        </is>
+      </c>
+      <c r="E1" t="inlineStr">
+        <is>
+          <t>3. O membro compromete-se com os resultados a alcançar de acordo com os objetivos estratégicos do departamento e júnior empresa, e é persistente perante obstáculos e dificuldades.</t>
+        </is>
+      </c>
+    </row>
+    <row r="2" ht="22.8" customHeight="1">
+      <c r="A2" t="inlineStr">
+        <is>
+          <t>Rafaela Carvalho</t>
+        </is>
+      </c>
+      <c r="B2" t="inlineStr">
+        <is>
+          <t>Catarina Milheiro</t>
+        </is>
+      </c>
+      <c r="C2" t="inlineStr">
+        <is>
+          <t>6</t>
+        </is>
+      </c>
+      <c r="D2" t="inlineStr">
+        <is>
+          <t>6</t>
+        </is>
+      </c>
+      <c r="E2" t="inlineStr">
+        <is>
+          <t>6</t>
+        </is>
+      </c>
+    </row>
+    <row r="3" ht="24" customHeight="1">
+      <c r="A3" t="inlineStr">
+        <is>
+          <t>Rafaela Carvalho</t>
+        </is>
+      </c>
+      <c r="B3" t="inlineStr">
+        <is>
+          <t>Gonçalo Figueiredo</t>
+        </is>
+      </c>
+      <c r="C3" t="inlineStr">
+        <is>
+          <t>5</t>
+        </is>
+      </c>
+      <c r="D3" t="inlineStr">
+        <is>
+          <t>5</t>
+        </is>
+      </c>
+      <c r="E3" t="inlineStr">
+        <is>
+          <t>5</t>
+        </is>
+      </c>
+    </row>
+    <row r="4" ht="21.6" customHeight="1">
+      <c r="A4" t="inlineStr">
+        <is>
+          <t>Rafaela Carvalho</t>
+        </is>
+      </c>
+      <c r="B4" t="inlineStr">
+        <is>
+          <t>Inês Cabral</t>
+        </is>
+      </c>
+      <c r="C4" t="inlineStr">
+        <is>
+          <t>5</t>
+        </is>
+      </c>
+      <c r="D4" t="inlineStr">
+        <is>
+          <t>5</t>
+        </is>
+      </c>
+      <c r="E4" t="inlineStr">
+        <is>
+          <t>5</t>
+        </is>
+      </c>
+    </row>
+    <row r="5" ht="22.8" customHeight="1">
+      <c r="A5" t="inlineStr">
+        <is>
+          <t>Paula Ferreira</t>
+        </is>
+      </c>
+      <c r="B5" t="inlineStr">
+        <is>
+          <t>Catarina Milheiro</t>
+        </is>
+      </c>
+      <c r="C5" t="inlineStr">
+        <is>
+          <t>6</t>
+        </is>
+      </c>
+      <c r="D5" t="inlineStr">
+        <is>
+          <t>6</t>
+        </is>
+      </c>
+      <c r="E5" t="inlineStr">
+        <is>
+          <t>6</t>
+        </is>
+      </c>
+    </row>
+    <row r="6" ht="24" customHeight="1">
+      <c r="A6" t="inlineStr">
+        <is>
+          <t>Paula Ferreira</t>
+        </is>
+      </c>
+      <c r="B6" t="inlineStr">
+        <is>
+          <t>Gonçalo Figueiredo</t>
+        </is>
+      </c>
+      <c r="C6" t="inlineStr">
+        <is>
+          <t>4</t>
+        </is>
+      </c>
+      <c r="D6" t="inlineStr">
+        <is>
+          <t>5</t>
+        </is>
+      </c>
+      <c r="E6" t="inlineStr">
+        <is>
+          <t>4</t>
+        </is>
+      </c>
+    </row>
+    <row r="7" ht="19.2" customHeight="1">
+      <c r="A7" t="inlineStr">
+        <is>
+          <t>Paula Ferreira</t>
+        </is>
+      </c>
+      <c r="B7" t="inlineStr">
+        <is>
+          <t>Inês Cabral</t>
+        </is>
+      </c>
+      <c r="C7" t="inlineStr">
+        <is>
+          <t>4</t>
+        </is>
+      </c>
+      <c r="D7" t="inlineStr">
+        <is>
+          <t>5</t>
+        </is>
+      </c>
+      <c r="E7" t="inlineStr">
+        <is>
+          <t>5</t>
+        </is>
+      </c>
+    </row>
+    <row r="8" ht="22.8" customHeight="1">
+      <c r="A8" t="inlineStr">
+        <is>
+          <t>Mariana Oliveira</t>
+        </is>
+      </c>
+      <c r="B8" t="inlineStr">
+        <is>
+          <t>Catarina Milheiro</t>
+        </is>
+      </c>
+      <c r="C8" t="inlineStr">
+        <is>
+          <t>6</t>
+        </is>
+      </c>
+      <c r="D8" t="inlineStr">
+        <is>
+          <t>6</t>
+        </is>
+      </c>
+      <c r="E8" t="inlineStr">
+        <is>
+          <t>6</t>
+        </is>
+      </c>
+    </row>
+    <row r="9" ht="24" customHeight="1">
+      <c r="A9" t="inlineStr">
+        <is>
+          <t>Mariana Oliveira</t>
+        </is>
+      </c>
+      <c r="B9" t="inlineStr">
+        <is>
+          <t>Gonçalo Figueiredo</t>
+        </is>
+      </c>
+      <c r="C9" t="inlineStr">
+        <is>
+          <t>3</t>
+        </is>
+      </c>
+      <c r="D9" t="inlineStr">
+        <is>
+          <t>2</t>
+        </is>
+      </c>
+      <c r="E9" t="inlineStr">
+        <is>
+          <t>2</t>
+        </is>
+      </c>
+    </row>
+    <row r="10" ht="21.6" customHeight="1">
+      <c r="A10" t="inlineStr">
+        <is>
+          <t>Mariana Oliveira</t>
+        </is>
+      </c>
+      <c r="B10" t="inlineStr">
+        <is>
+          <t>Inês Cabral</t>
+        </is>
+      </c>
+      <c r="C10" t="inlineStr">
+        <is>
+          <t>5</t>
+        </is>
+      </c>
+      <c r="D10" t="inlineStr">
+        <is>
+          <t>5</t>
+        </is>
+      </c>
+      <c r="E10" t="inlineStr">
+        <is>
+          <t>6</t>
+        </is>
+      </c>
+    </row>
+    <row r="11" ht="22.8" customHeight="1">
+      <c r="A11" t="inlineStr">
+        <is>
+          <t>Inês Cabral</t>
+        </is>
+      </c>
+      <c r="B11" t="inlineStr">
+        <is>
+          <t>Catarina Milheiro</t>
+        </is>
+      </c>
+      <c r="C11" t="inlineStr">
+        <is>
+          <t>6</t>
+        </is>
+      </c>
+      <c r="D11" t="inlineStr">
+        <is>
+          <t>6</t>
+        </is>
+      </c>
+      <c r="E11" t="inlineStr">
+        <is>
+          <t>6</t>
+        </is>
+      </c>
+    </row>
+    <row r="12" ht="24" customHeight="1">
+      <c r="A12" t="inlineStr">
+        <is>
+          <t>Inês Cabral</t>
+        </is>
+      </c>
+      <c r="B12" t="inlineStr">
+        <is>
+          <t>Gonçalo Figueiredo</t>
+        </is>
+      </c>
+      <c r="C12" t="inlineStr">
+        <is>
+          <t>6</t>
+        </is>
+      </c>
+      <c r="D12" t="inlineStr">
+        <is>
+          <t>4</t>
+        </is>
+      </c>
+      <c r="E12" t="inlineStr">
+        <is>
+          <t>4</t>
+        </is>
+      </c>
+    </row>
+    <row r="13" ht="15.6" customHeight="1">
+      <c r="A13" t="inlineStr">
+        <is>
+          <t>Inês Cabral</t>
+        </is>
+      </c>
+      <c r="B13" t="inlineStr">
+        <is>
+          <t>Inês Cabral</t>
+        </is>
+      </c>
+      <c r="C13" t="inlineStr">
+        <is>
+          <t>6</t>
+        </is>
+      </c>
+      <c r="D13" t="inlineStr">
+        <is>
+          <t>5</t>
+        </is>
+      </c>
+      <c r="E13" t="inlineStr">
+        <is>
+          <t>6</t>
+        </is>
+      </c>
+    </row>
+    <row r="14" ht="22.8" customHeight="1">
+      <c r="A14" t="inlineStr">
+        <is>
+          <t>Mariana Arezes</t>
+        </is>
+      </c>
+      <c r="B14" t="inlineStr">
+        <is>
+          <t>Catarina Milheiro</t>
+        </is>
+      </c>
+      <c r="C14" t="inlineStr">
+        <is>
+          <t>6</t>
+        </is>
+      </c>
+      <c r="D14" t="inlineStr">
+        <is>
+          <t>5</t>
+        </is>
+      </c>
+      <c r="E14" t="inlineStr">
+        <is>
+          <t>6</t>
+        </is>
+      </c>
+    </row>
+    <row r="15" ht="24" customHeight="1">
+      <c r="A15" t="inlineStr">
+        <is>
+          <t>Mariana Arezes</t>
+        </is>
+      </c>
+      <c r="B15" t="inlineStr">
+        <is>
+          <t>Gonçalo Figueiredo</t>
+        </is>
+      </c>
+      <c r="C15" t="inlineStr">
+        <is>
+          <t>5</t>
+        </is>
+      </c>
+      <c r="D15" t="inlineStr">
+        <is>
+          <t>5</t>
+        </is>
+      </c>
+      <c r="E15" t="inlineStr">
+        <is>
+          <t>5</t>
+        </is>
+      </c>
+    </row>
+    <row r="16" ht="19.2" customHeight="1">
+      <c r="A16" t="inlineStr">
+        <is>
+          <t>Mariana Arezes</t>
+        </is>
+      </c>
+      <c r="B16" t="inlineStr">
+        <is>
+          <t>Inês Cabral</t>
+        </is>
+      </c>
+      <c r="C16" t="inlineStr">
+        <is>
+          <t>6</t>
+        </is>
+      </c>
+      <c r="D16" t="inlineStr">
+        <is>
+          <t>5</t>
+        </is>
+      </c>
+      <c r="E16" t="inlineStr">
+        <is>
+          <t>5</t>
+        </is>
+      </c>
+    </row>
+    <row r="17" ht="22.8" customHeight="1">
+      <c r="A17" t="inlineStr">
+        <is>
+          <t>Paulo Vieira</t>
+        </is>
+      </c>
+      <c r="B17" t="inlineStr">
+        <is>
+          <t>Catarina Milheiro</t>
+        </is>
+      </c>
+      <c r="C17" t="inlineStr">
+        <is>
+          <t>6</t>
+        </is>
+      </c>
+      <c r="D17" t="inlineStr">
+        <is>
+          <t>6</t>
+        </is>
+      </c>
+      <c r="E17" t="inlineStr">
+        <is>
+          <t>6</t>
+        </is>
+      </c>
+    </row>
+    <row r="18" ht="24" customHeight="1">
+      <c r="A18" t="inlineStr">
+        <is>
+          <t>Paulo Vieira</t>
+        </is>
+      </c>
+      <c r="B18" t="inlineStr">
+        <is>
+          <t>Gonçalo Figueiredo</t>
+        </is>
+      </c>
+      <c r="C18" t="inlineStr">
+        <is>
+          <t>5</t>
+        </is>
+      </c>
+      <c r="D18" t="inlineStr">
+        <is>
+          <t>4</t>
+        </is>
+      </c>
+      <c r="E18" t="inlineStr">
+        <is>
+          <t>4</t>
+        </is>
+      </c>
+    </row>
+    <row r="19" ht="16.8" customHeight="1">
+      <c r="A19" t="inlineStr">
+        <is>
+          <t>Paulo Vieira</t>
+        </is>
+      </c>
+      <c r="B19" t="inlineStr">
+        <is>
+          <t>Inês Cabral</t>
+        </is>
+      </c>
+      <c r="C19" t="inlineStr">
+        <is>
+          <t>5</t>
+        </is>
+      </c>
+      <c r="D19" t="inlineStr">
+        <is>
+          <t>4</t>
+        </is>
+      </c>
+      <c r="E19" t="inlineStr">
+        <is>
+          <t>4</t>
+        </is>
+      </c>
+    </row>
+    <row r="20" ht="24" customHeight="1">
+      <c r="A20" t="inlineStr">
+        <is>
+          <t>Gonçalo Figueiredo</t>
+        </is>
+      </c>
+      <c r="B20" t="inlineStr">
+        <is>
+          <t>Catarina Milheiro</t>
+        </is>
+      </c>
+      <c r="C20" t="inlineStr">
+        <is>
+          <t>6</t>
+        </is>
+      </c>
+      <c r="D20" t="inlineStr">
+        <is>
+          <t>6</t>
+        </is>
+      </c>
+      <c r="E20" t="inlineStr">
+        <is>
+          <t>6</t>
+        </is>
+      </c>
+    </row>
+    <row r="21" ht="24" customHeight="1">
+      <c r="A21" t="inlineStr">
+        <is>
+          <t>Gonçalo Figueiredo</t>
+        </is>
+      </c>
+      <c r="B21" t="inlineStr">
+        <is>
+          <t>Gonçalo Figueiredo</t>
+        </is>
+      </c>
+      <c r="C21" t="inlineStr">
+        <is>
+          <t>4</t>
+        </is>
+      </c>
+      <c r="D21" t="inlineStr">
+        <is>
+          <t>4</t>
+        </is>
+      </c>
+      <c r="E21" t="inlineStr">
+        <is>
+          <t>5</t>
+        </is>
+      </c>
+    </row>
+    <row r="22" ht="24" customHeight="1">
+      <c r="A22" t="inlineStr">
+        <is>
+          <t>Gonçalo Figueiredo</t>
+        </is>
+      </c>
+      <c r="B22" t="inlineStr">
+        <is>
+          <t>Inês Cabral</t>
+        </is>
+      </c>
+      <c r="C22" t="inlineStr">
+        <is>
+          <t>6</t>
+        </is>
+      </c>
+      <c r="D22" t="inlineStr">
+        <is>
+          <t>6</t>
+        </is>
+      </c>
+      <c r="E22" t="inlineStr">
+        <is>
+          <t>6</t>
+        </is>
+      </c>
+    </row>
+    <row r="23" ht="22.8" customHeight="1">
+      <c r="A23" t="inlineStr">
+        <is>
+          <t>Catarina Milheiro</t>
+        </is>
+      </c>
+      <c r="B23" t="inlineStr">
+        <is>
+          <t>Catarina Milheiro</t>
+        </is>
+      </c>
+      <c r="C23" t="inlineStr">
+        <is>
+          <t>6</t>
+        </is>
+      </c>
+      <c r="D23" t="inlineStr">
+        <is>
+          <t>6</t>
+        </is>
+      </c>
+      <c r="E23" t="inlineStr">
+        <is>
+          <t>6</t>
+        </is>
+      </c>
+    </row>
+    <row r="24" ht="24" customHeight="1">
+      <c r="A24" t="inlineStr">
+        <is>
+          <t>Catarina Milheiro</t>
+        </is>
+      </c>
+      <c r="B24" t="inlineStr">
+        <is>
+          <t>Gonçalo Figueiredo</t>
+        </is>
+      </c>
+      <c r="C24" t="inlineStr">
+        <is>
+          <t>4</t>
+        </is>
+      </c>
+      <c r="D24" t="inlineStr">
+        <is>
+          <t>4</t>
+        </is>
+      </c>
+      <c r="E24" t="inlineStr">
+        <is>
+          <t>4</t>
+        </is>
+      </c>
+    </row>
+    <row r="25" ht="22.8" customHeight="1">
+      <c r="A25" t="inlineStr">
+        <is>
+          <t>Catarina Milheiro</t>
+        </is>
+      </c>
+      <c r="B25" t="inlineStr">
+        <is>
+          <t>Inês Cabral</t>
+        </is>
+      </c>
+      <c r="C25" t="inlineStr">
+        <is>
+          <t>4</t>
+        </is>
+      </c>
+      <c r="D25" t="inlineStr">
+        <is>
+          <t>4</t>
+        </is>
+      </c>
+      <c r="E25" t="inlineStr">
+        <is>
+          <t>4</t>
+        </is>
+      </c>
+    </row>
+    <row r="26" ht="22.8" customHeight="1">
+      <c r="A26" t="inlineStr">
+        <is>
+          <t>Inês Bastos</t>
+        </is>
+      </c>
+      <c r="B26" t="inlineStr">
+        <is>
+          <t>Catarina Milheiro</t>
+        </is>
+      </c>
+      <c r="C26" t="inlineStr">
+        <is>
+          <t>6</t>
+        </is>
+      </c>
+      <c r="D26" t="inlineStr">
+        <is>
+          <t>6</t>
+        </is>
+      </c>
+      <c r="E26" t="inlineStr">
+        <is>
+          <t>6</t>
+        </is>
+      </c>
+    </row>
+    <row r="27" ht="24" customHeight="1">
+      <c r="A27" t="inlineStr">
+        <is>
+          <t>Inês Bastos</t>
+        </is>
+      </c>
+      <c r="B27" t="inlineStr">
+        <is>
+          <t>Gonçalo Figueiredo</t>
+        </is>
+      </c>
+      <c r="C27" t="inlineStr">
+        <is>
+          <t>4</t>
+        </is>
+      </c>
+      <c r="D27" t="inlineStr">
+        <is>
+          <t>3</t>
+        </is>
+      </c>
+      <c r="E27" t="inlineStr">
+        <is>
+          <t>5</t>
+        </is>
+      </c>
+    </row>
+    <row r="28" ht="15.6" customHeight="1">
+      <c r="A28" t="inlineStr">
+        <is>
+          <t>Inês Bastos</t>
+        </is>
+      </c>
+      <c r="B28" t="inlineStr">
+        <is>
+          <t>Inês Cabral</t>
+        </is>
+      </c>
+      <c r="C28" t="inlineStr">
+        <is>
+          <t>4</t>
+        </is>
+      </c>
+      <c r="D28" t="inlineStr">
+        <is>
+          <t>4</t>
+        </is>
+      </c>
+      <c r="E28" t="inlineStr">
+        <is>
+          <t>5</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
so falta colocar os estilos a funcionar direito
</commit_message>
<xml_diff>
--- a/output/Output-Avaliacao-Membro-RH.xlsx
+++ b/output/Output-Avaliacao-Membro-RH.xlsx
@@ -413,7 +413,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:H87"/>
+  <dimension ref="A1:H152"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -434,6 +434,11 @@
           <t>Avaliador</t>
         </is>
       </c>
+      <c r="B2" t="inlineStr">
+        <is>
+          <t>Avaliador</t>
+        </is>
+      </c>
       <c r="C2" t="inlineStr">
         <is>
           <t>Avaliado</t>
@@ -456,6 +461,11 @@
       </c>
     </row>
     <row r="3">
+      <c r="A3" t="inlineStr">
+        <is>
+          <t>Avaliador</t>
+        </is>
+      </c>
       <c r="C3" t="inlineStr">
         <is>
           <t>Avaliado</t>
@@ -478,120 +488,105 @@
       </c>
     </row>
     <row r="4">
-      <c r="A4" t="inlineStr">
+      <c r="C4" t="inlineStr">
+        <is>
+          <t>Catarina Milheiro</t>
+        </is>
+      </c>
+      <c r="D4" t="inlineStr">
+        <is>
+          <t>Catarina Milheiro</t>
+        </is>
+      </c>
+      <c r="E4" t="n">
+        <v>6</v>
+      </c>
+      <c r="F4" t="n">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="inlineStr">
         <is>
           <t>Rafaela Carvalho</t>
         </is>
       </c>
-      <c r="B4" t="inlineStr">
+      <c r="B5" t="inlineStr">
         <is>
           <t>Rafaela Carvalho</t>
         </is>
       </c>
-      <c r="C4" t="inlineStr">
-        <is>
-          <t>Catarina Milheiro</t>
-        </is>
-      </c>
-      <c r="D4" t="inlineStr">
-        <is>
-          <t>Catarina Milheiro</t>
-        </is>
-      </c>
-      <c r="E4" t="n">
-        <v>6</v>
-      </c>
-      <c r="F4" t="n">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="5">
-      <c r="B5" t="inlineStr">
+      <c r="C5" t="inlineStr">
+        <is>
+          <t>Catarina Milheiro</t>
+        </is>
+      </c>
+      <c r="D5" t="inlineStr">
+        <is>
+          <t>Catarina Milheiro</t>
+        </is>
+      </c>
+      <c r="E5" t="n">
+        <v>6</v>
+      </c>
+      <c r="F5" t="n">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="B6" t="inlineStr">
         <is>
           <t>Rafaela Carvalho</t>
         </is>
       </c>
-      <c r="C5" t="inlineStr">
-        <is>
-          <t>Gonçalo Figueiredo</t>
-        </is>
-      </c>
-      <c r="D5" t="inlineStr">
-        <is>
-          <t>Gonçalo Figueiredo</t>
-        </is>
-      </c>
-      <c r="E5" t="n">
-        <v>5</v>
-      </c>
-      <c r="F5" t="n">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="6">
-      <c r="A6" t="inlineStr">
+      <c r="C6" t="inlineStr">
+        <is>
+          <t>Gonçalo Figueiredo</t>
+        </is>
+      </c>
+      <c r="D6" t="inlineStr">
+        <is>
+          <t>Gonçalo Figueiredo</t>
+        </is>
+      </c>
+      <c r="E6" t="n">
+        <v>5</v>
+      </c>
+      <c r="F6" t="n">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="inlineStr">
         <is>
           <t>Rafaela Carvalho</t>
         </is>
       </c>
-      <c r="B6" t="inlineStr">
+      <c r="B7" t="inlineStr">
         <is>
           <t>Rafaela Carvalho</t>
         </is>
       </c>
-      <c r="D6" t="inlineStr">
-        <is>
-          <t>Inês Cabral</t>
-        </is>
-      </c>
-      <c r="E6" t="n">
-        <v>5</v>
-      </c>
-      <c r="F6" t="n">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="7">
-      <c r="C7" t="inlineStr">
-        <is>
-          <t>Catarina Milheiro</t>
-        </is>
-      </c>
       <c r="D7" t="inlineStr">
         <is>
-          <t>Catarina Milheiro</t>
+          <t>Gonçalo Figueiredo</t>
         </is>
       </c>
       <c r="E7" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F7" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="8">
-      <c r="A8" t="inlineStr">
-        <is>
-          <t>Paula Ferreira</t>
-        </is>
-      </c>
-      <c r="B8" t="inlineStr">
-        <is>
-          <t>Paula Ferreira</t>
-        </is>
-      </c>
-      <c r="C8" t="inlineStr">
-        <is>
-          <t>Gonçalo Figueiredo</t>
-        </is>
-      </c>
       <c r="D8" t="inlineStr">
         <is>
-          <t>Gonçalo Figueiredo</t>
+          <t>Inês Cabral</t>
         </is>
       </c>
       <c r="E8" t="n">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="F8" t="n">
         <v>5</v>
@@ -600,12 +595,7 @@
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>Paula Ferreira</t>
-        </is>
-      </c>
-      <c r="B9" t="inlineStr">
-        <is>
-          <t>Paula Ferreira</t>
+          <t>Rafaela Carvalho</t>
         </is>
       </c>
       <c r="D9" t="inlineStr">
@@ -614,7 +604,7 @@
         </is>
       </c>
       <c r="E9" t="n">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="F9" t="n">
         <v>5</v>
@@ -623,12 +613,7 @@
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>Mariana Oliveira</t>
-        </is>
-      </c>
-      <c r="B10" t="inlineStr">
-        <is>
-          <t>Mariana Oliveira</t>
+          <t>Paula Ferreira</t>
         </is>
       </c>
       <c r="D10" t="inlineStr">
@@ -646,49 +631,39 @@
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>Mariana Oliveira</t>
-        </is>
-      </c>
-      <c r="B11" t="inlineStr">
-        <is>
-          <t>Mariana Oliveira</t>
+          <t>Paula Ferreira</t>
         </is>
       </c>
       <c r="C11" t="inlineStr">
         <is>
-          <t>Gonçalo Figueiredo</t>
+          <t>Catarina Milheiro</t>
         </is>
       </c>
       <c r="D11" t="inlineStr">
         <is>
-          <t>Gonçalo Figueiredo</t>
+          <t>Catarina Milheiro</t>
         </is>
       </c>
       <c r="E11" t="n">
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="F11" t="n">
-        <v>2</v>
+        <v>6</v>
       </c>
     </row>
     <row r="12">
-      <c r="A12" t="inlineStr">
-        <is>
-          <t>Mariana Oliveira</t>
-        </is>
-      </c>
-      <c r="B12" t="inlineStr">
-        <is>
-          <t>Mariana Oliveira</t>
+      <c r="C12" t="inlineStr">
+        <is>
+          <t>Gonçalo Figueiredo</t>
         </is>
       </c>
       <c r="D12" t="inlineStr">
         <is>
-          <t>Inês Cabral</t>
+          <t>Gonçalo Figueiredo</t>
         </is>
       </c>
       <c r="E12" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F12" t="n">
         <v>5</v>
@@ -697,211 +672,191 @@
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
-          <t>Inês Cabral</t>
+          <t>Paula Ferreira</t>
         </is>
       </c>
       <c r="B13" t="inlineStr">
         <is>
-          <t>Inês Cabral</t>
+          <t>Paula Ferreira</t>
+        </is>
+      </c>
+      <c r="C13" t="inlineStr">
+        <is>
+          <t>Gonçalo Figueiredo</t>
         </is>
       </c>
       <c r="D13" t="inlineStr">
         <is>
-          <t>Catarina Milheiro</t>
+          <t>Gonçalo Figueiredo</t>
         </is>
       </c>
       <c r="E13" t="n">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="F13" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="14">
-      <c r="A14" t="inlineStr">
-        <is>
-          <t>Inês Cabral</t>
-        </is>
-      </c>
       <c r="B14" t="inlineStr">
         <is>
-          <t>Inês Cabral</t>
+          <t>Paula Ferreira</t>
         </is>
       </c>
       <c r="C14" t="inlineStr">
         <is>
-          <t>Gonçalo Figueiredo</t>
+          <t>Inês Cabral</t>
         </is>
       </c>
       <c r="D14" t="inlineStr">
         <is>
-          <t>Gonçalo Figueiredo</t>
+          <t>Inês Cabral</t>
         </is>
       </c>
       <c r="E14" t="n">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="F14" t="n">
-        <v>4</v>
+        <v>5</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="inlineStr">
         <is>
-          <t>Inês Cabral</t>
+          <t>Paula Ferreira</t>
         </is>
       </c>
       <c r="B15" t="inlineStr">
         <is>
-          <t>Inês Cabral</t>
-        </is>
-      </c>
-      <c r="D15" t="inlineStr">
+          <t>Paula Ferreira</t>
+        </is>
+      </c>
+      <c r="C15" t="inlineStr">
         <is>
           <t>Inês Cabral</t>
         </is>
       </c>
       <c r="E15" t="n">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="F15" t="n">
         <v>5</v>
       </c>
     </row>
     <row r="16">
-      <c r="A16" t="inlineStr">
-        <is>
-          <t>Mariana Arezes</t>
-        </is>
-      </c>
-      <c r="C16" t="inlineStr">
-        <is>
-          <t>Catarina Milheiro</t>
-        </is>
-      </c>
-      <c r="D16" t="inlineStr">
-        <is>
-          <t>Catarina Milheiro</t>
+      <c r="B16" t="inlineStr">
+        <is>
+          <t>Mariana Oliveira</t>
         </is>
       </c>
       <c r="E16" t="n">
         <v>6</v>
       </c>
       <c r="F16" t="n">
-        <v>5</v>
+        <v>6</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="inlineStr">
         <is>
-          <t>Mariana Arezes</t>
+          <t>Mariana Oliveira</t>
         </is>
       </c>
       <c r="B17" t="inlineStr">
         <is>
-          <t>Mariana Arezes</t>
+          <t>Mariana Oliveira</t>
         </is>
       </c>
       <c r="C17" t="inlineStr">
         <is>
-          <t>Gonçalo Figueiredo</t>
+          <t>Catarina Milheiro</t>
         </is>
       </c>
       <c r="D17" t="inlineStr">
         <is>
-          <t>Gonçalo Figueiredo</t>
+          <t>Catarina Milheiro</t>
         </is>
       </c>
       <c r="E17" t="n">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="F17" t="n">
-        <v>5</v>
+        <v>6</v>
       </c>
     </row>
     <row r="18">
-      <c r="A18" t="inlineStr">
-        <is>
-          <t>Mariana Arezes</t>
-        </is>
-      </c>
       <c r="B18" t="inlineStr">
         <is>
-          <t>Mariana Arezes</t>
+          <t>Mariana Oliveira</t>
+        </is>
+      </c>
+      <c r="C18" t="inlineStr">
+        <is>
+          <t>Gonçalo Figueiredo</t>
         </is>
       </c>
       <c r="D18" t="inlineStr">
         <is>
-          <t>Inês Cabral</t>
+          <t>Gonçalo Figueiredo</t>
         </is>
       </c>
       <c r="E18" t="n">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="F18" t="n">
-        <v>5</v>
+        <v>2</v>
       </c>
     </row>
     <row r="19">
       <c r="A19" t="inlineStr">
         <is>
-          <t>Paulo Vieira</t>
+          <t>Mariana Oliveira</t>
         </is>
       </c>
       <c r="B19" t="inlineStr">
         <is>
-          <t>Paulo Vieira</t>
-        </is>
-      </c>
-      <c r="D19" t="inlineStr">
-        <is>
-          <t>Catarina Milheiro</t>
+          <t>Mariana Oliveira</t>
+        </is>
+      </c>
+      <c r="C19" t="inlineStr">
+        <is>
+          <t>Gonçalo Figueiredo</t>
         </is>
       </c>
       <c r="E19" t="n">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="F19" t="n">
-        <v>6</v>
+        <v>2</v>
       </c>
     </row>
     <row r="20">
-      <c r="A20" t="inlineStr">
-        <is>
-          <t>Paulo Vieira</t>
-        </is>
-      </c>
       <c r="B20" t="inlineStr">
         <is>
-          <t>Paulo Vieira</t>
-        </is>
-      </c>
-      <c r="C20" t="inlineStr">
-        <is>
-          <t>Gonçalo Figueiredo</t>
-        </is>
-      </c>
-      <c r="D20" t="inlineStr">
-        <is>
-          <t>Gonçalo Figueiredo</t>
+          <t>Mariana Oliveira</t>
         </is>
       </c>
       <c r="E20" t="n">
         <v>5</v>
       </c>
       <c r="F20" t="n">
-        <v>4</v>
+        <v>5</v>
       </c>
     </row>
     <row r="21">
       <c r="A21" t="inlineStr">
         <is>
-          <t>Paulo Vieira</t>
+          <t>Mariana Oliveira</t>
         </is>
       </c>
       <c r="B21" t="inlineStr">
         <is>
-          <t>Paulo Vieira</t>
+          <t>Mariana Oliveira</t>
+        </is>
+      </c>
+      <c r="C21" t="inlineStr">
+        <is>
+          <t>Inês Cabral</t>
         </is>
       </c>
       <c r="D21" t="inlineStr">
@@ -913,18 +868,18 @@
         <v>5</v>
       </c>
       <c r="F21" t="n">
-        <v>4</v>
+        <v>5</v>
       </c>
     </row>
     <row r="22">
-      <c r="A22" t="inlineStr">
-        <is>
-          <t>Gonçalo Figueiredo</t>
-        </is>
-      </c>
       <c r="B22" t="inlineStr">
         <is>
-          <t>Gonçalo Figueiredo</t>
+          <t>Inês Cabral</t>
+        </is>
+      </c>
+      <c r="C22" t="inlineStr">
+        <is>
+          <t>Catarina Milheiro</t>
         </is>
       </c>
       <c r="D22" t="inlineStr">
@@ -942,114 +897,84 @@
     <row r="23">
       <c r="A23" t="inlineStr">
         <is>
-          <t>Gonçalo Figueiredo</t>
+          <t>Inês Cabral</t>
         </is>
       </c>
       <c r="B23" t="inlineStr">
         <is>
-          <t>Gonçalo Figueiredo</t>
-        </is>
-      </c>
-      <c r="C23" t="inlineStr">
-        <is>
-          <t>Gonçalo Figueiredo</t>
+          <t>Inês Cabral</t>
         </is>
       </c>
       <c r="D23" t="inlineStr">
         <is>
-          <t>Gonçalo Figueiredo</t>
+          <t>Catarina Milheiro</t>
         </is>
       </c>
       <c r="E23" t="n">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="F23" t="n">
-        <v>4</v>
+        <v>6</v>
       </c>
     </row>
     <row r="24">
-      <c r="A24" t="inlineStr">
-        <is>
-          <t>Gonçalo Figueiredo</t>
-        </is>
-      </c>
-      <c r="B24" t="inlineStr">
-        <is>
-          <t>Gonçalo Figueiredo</t>
-        </is>
-      </c>
       <c r="D24" t="inlineStr">
         <is>
-          <t>Inês Cabral</t>
+          <t>Gonçalo Figueiredo</t>
         </is>
       </c>
       <c r="E24" t="n">
         <v>6</v>
       </c>
       <c r="F24" t="n">
-        <v>6</v>
+        <v>4</v>
       </c>
     </row>
     <row r="25">
       <c r="A25" t="inlineStr">
         <is>
-          <t>Catarina Milheiro</t>
-        </is>
-      </c>
-      <c r="C25" t="inlineStr">
-        <is>
-          <t>Catarina Milheiro</t>
+          <t>Inês Cabral</t>
         </is>
       </c>
       <c r="D25" t="inlineStr">
         <is>
-          <t>Catarina Milheiro</t>
+          <t>Gonçalo Figueiredo</t>
         </is>
       </c>
       <c r="E25" t="n">
         <v>6</v>
       </c>
       <c r="F25" t="n">
-        <v>6</v>
+        <v>4</v>
       </c>
     </row>
     <row r="26">
       <c r="A26" t="inlineStr">
         <is>
-          <t>Catarina Milheiro</t>
-        </is>
-      </c>
-      <c r="B26" t="inlineStr">
-        <is>
-          <t>Catarina Milheiro</t>
-        </is>
-      </c>
-      <c r="C26" t="inlineStr">
-        <is>
-          <t>Gonçalo Figueiredo</t>
+          <t>Inês Cabral</t>
         </is>
       </c>
       <c r="D26" t="inlineStr">
         <is>
-          <t>Gonçalo Figueiredo</t>
+          <t>Inês Cabral</t>
         </is>
       </c>
       <c r="E26" t="n">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="F26" t="n">
-        <v>4</v>
+        <v>5</v>
       </c>
     </row>
     <row r="27">
       <c r="A27" t="inlineStr">
         <is>
-          <t>Catarina Milheiro</t>
-        </is>
-      </c>
-      <c r="B27" t="inlineStr">
-        <is>
-          <t>Catarina Milheiro</t>
+          <t>Inês Cabral</t>
+        </is>
+      </c>
+      <c r="C27" t="inlineStr">
+        <is>
+          <t>Inês Cabral</t>
         </is>
       </c>
       <c r="D27" t="inlineStr">
@@ -1058,21 +983,16 @@
         </is>
       </c>
       <c r="E27" t="n">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="F27" t="n">
-        <v>4</v>
+        <v>5</v>
       </c>
     </row>
     <row r="28">
-      <c r="A28" t="inlineStr">
-        <is>
-          <t>Inês Bastos</t>
-        </is>
-      </c>
-      <c r="B28" t="inlineStr">
-        <is>
-          <t>Inês Bastos</t>
+      <c r="C28" t="inlineStr">
+        <is>
+          <t>Catarina Milheiro</t>
         </is>
       </c>
       <c r="D28" t="inlineStr">
@@ -1084,87 +1004,626 @@
         <v>6</v>
       </c>
       <c r="F28" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="29">
       <c r="A29" t="inlineStr">
         <is>
+          <t>Mariana Arezes</t>
+        </is>
+      </c>
+      <c r="B29" t="inlineStr">
+        <is>
+          <t>Mariana Arezes</t>
+        </is>
+      </c>
+      <c r="C29" t="inlineStr">
+        <is>
+          <t>Catarina Milheiro</t>
+        </is>
+      </c>
+      <c r="D29" t="inlineStr">
+        <is>
+          <t>Catarina Milheiro</t>
+        </is>
+      </c>
+      <c r="E29" t="n">
+        <v>6</v>
+      </c>
+      <c r="F29" t="n">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="30">
+      <c r="B30" t="inlineStr">
+        <is>
+          <t>Mariana Arezes</t>
+        </is>
+      </c>
+      <c r="C30" t="inlineStr">
+        <is>
+          <t>Gonçalo Figueiredo</t>
+        </is>
+      </c>
+      <c r="D30" t="inlineStr">
+        <is>
+          <t>Gonçalo Figueiredo</t>
+        </is>
+      </c>
+      <c r="E30" t="n">
+        <v>5</v>
+      </c>
+      <c r="F30" t="n">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="31">
+      <c r="A31" t="inlineStr">
+        <is>
+          <t>Mariana Arezes</t>
+        </is>
+      </c>
+      <c r="B31" t="inlineStr">
+        <is>
+          <t>Mariana Arezes</t>
+        </is>
+      </c>
+      <c r="C31" t="inlineStr">
+        <is>
+          <t>Gonçalo Figueiredo</t>
+        </is>
+      </c>
+      <c r="E31" t="n">
+        <v>5</v>
+      </c>
+      <c r="F31" t="n">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="32">
+      <c r="B32" t="inlineStr">
+        <is>
+          <t>Mariana Arezes</t>
+        </is>
+      </c>
+      <c r="E32" t="n">
+        <v>6</v>
+      </c>
+      <c r="F32" t="n">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="33">
+      <c r="A33" t="inlineStr">
+        <is>
+          <t>Mariana Arezes</t>
+        </is>
+      </c>
+      <c r="B33" t="inlineStr">
+        <is>
+          <t>Mariana Arezes</t>
+        </is>
+      </c>
+      <c r="C33" t="inlineStr">
+        <is>
+          <t>Inês Cabral</t>
+        </is>
+      </c>
+      <c r="D33" t="inlineStr">
+        <is>
+          <t>Inês Cabral</t>
+        </is>
+      </c>
+      <c r="E33" t="n">
+        <v>6</v>
+      </c>
+      <c r="F33" t="n">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="34">
+      <c r="B34" t="inlineStr">
+        <is>
+          <t>Paulo Vieira</t>
+        </is>
+      </c>
+      <c r="C34" t="inlineStr">
+        <is>
+          <t>Catarina Milheiro</t>
+        </is>
+      </c>
+      <c r="D34" t="inlineStr">
+        <is>
+          <t>Catarina Milheiro</t>
+        </is>
+      </c>
+      <c r="E34" t="n">
+        <v>6</v>
+      </c>
+      <c r="F34" t="n">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="35">
+      <c r="A35" t="inlineStr">
+        <is>
+          <t>Paulo Vieira</t>
+        </is>
+      </c>
+      <c r="B35" t="inlineStr">
+        <is>
+          <t>Paulo Vieira</t>
+        </is>
+      </c>
+      <c r="C35" t="inlineStr">
+        <is>
+          <t>Catarina Milheiro</t>
+        </is>
+      </c>
+      <c r="E35" t="n">
+        <v>6</v>
+      </c>
+      <c r="F35" t="n">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="36">
+      <c r="B36" t="inlineStr">
+        <is>
+          <t>Paulo Vieira</t>
+        </is>
+      </c>
+      <c r="E36" t="n">
+        <v>5</v>
+      </c>
+      <c r="F36" t="n">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="37">
+      <c r="A37" t="inlineStr">
+        <is>
+          <t>Paulo Vieira</t>
+        </is>
+      </c>
+      <c r="B37" t="inlineStr">
+        <is>
+          <t>Paulo Vieira</t>
+        </is>
+      </c>
+      <c r="C37" t="inlineStr">
+        <is>
+          <t>Gonçalo Figueiredo</t>
+        </is>
+      </c>
+      <c r="D37" t="inlineStr">
+        <is>
+          <t>Gonçalo Figueiredo</t>
+        </is>
+      </c>
+      <c r="E37" t="n">
+        <v>5</v>
+      </c>
+      <c r="F37" t="n">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="38">
+      <c r="B38" t="inlineStr">
+        <is>
+          <t>Paulo Vieira</t>
+        </is>
+      </c>
+      <c r="C38" t="inlineStr">
+        <is>
+          <t>Inês Cabral</t>
+        </is>
+      </c>
+      <c r="D38" t="inlineStr">
+        <is>
+          <t>Inês Cabral</t>
+        </is>
+      </c>
+      <c r="E38" t="n">
+        <v>5</v>
+      </c>
+      <c r="F38" t="n">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="39">
+      <c r="A39" t="inlineStr">
+        <is>
+          <t>Paulo Vieira</t>
+        </is>
+      </c>
+      <c r="B39" t="inlineStr">
+        <is>
+          <t>Paulo Vieira</t>
+        </is>
+      </c>
+      <c r="D39" t="inlineStr">
+        <is>
+          <t>Inês Cabral</t>
+        </is>
+      </c>
+      <c r="E39" t="n">
+        <v>5</v>
+      </c>
+      <c r="F39" t="n">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="40">
+      <c r="D40" t="inlineStr">
+        <is>
+          <t>Catarina Milheiro</t>
+        </is>
+      </c>
+      <c r="E40" t="n">
+        <v>6</v>
+      </c>
+      <c r="F40" t="n">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="41">
+      <c r="A41" t="inlineStr">
+        <is>
+          <t>Gonçalo Figueiredo</t>
+        </is>
+      </c>
+      <c r="D41" t="inlineStr">
+        <is>
+          <t>Catarina Milheiro</t>
+        </is>
+      </c>
+      <c r="E41" t="n">
+        <v>6</v>
+      </c>
+      <c r="F41" t="n">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="42">
+      <c r="A42" t="inlineStr">
+        <is>
+          <t>Gonçalo Figueiredo</t>
+        </is>
+      </c>
+      <c r="D42" t="inlineStr">
+        <is>
+          <t>Gonçalo Figueiredo</t>
+        </is>
+      </c>
+      <c r="E42" t="n">
+        <v>4</v>
+      </c>
+      <c r="F42" t="n">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="43">
+      <c r="A43" t="inlineStr">
+        <is>
+          <t>Gonçalo Figueiredo</t>
+        </is>
+      </c>
+      <c r="C43" t="inlineStr">
+        <is>
+          <t>Gonçalo Figueiredo</t>
+        </is>
+      </c>
+      <c r="D43" t="inlineStr">
+        <is>
+          <t>Gonçalo Figueiredo</t>
+        </is>
+      </c>
+      <c r="E43" t="n">
+        <v>4</v>
+      </c>
+      <c r="F43" t="n">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="44">
+      <c r="C44" t="inlineStr">
+        <is>
+          <t>Inês Cabral</t>
+        </is>
+      </c>
+      <c r="D44" t="inlineStr">
+        <is>
+          <t>Inês Cabral</t>
+        </is>
+      </c>
+      <c r="E44" t="n">
+        <v>6</v>
+      </c>
+      <c r="F44" t="n">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="45">
+      <c r="A45" t="inlineStr">
+        <is>
+          <t>Gonçalo Figueiredo</t>
+        </is>
+      </c>
+      <c r="B45" t="inlineStr">
+        <is>
+          <t>Gonçalo Figueiredo</t>
+        </is>
+      </c>
+      <c r="C45" t="inlineStr">
+        <is>
+          <t>Inês Cabral</t>
+        </is>
+      </c>
+      <c r="D45" t="inlineStr">
+        <is>
+          <t>Inês Cabral</t>
+        </is>
+      </c>
+      <c r="E45" t="n">
+        <v>6</v>
+      </c>
+      <c r="F45" t="n">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="46">
+      <c r="B46" t="inlineStr">
+        <is>
+          <t>Catarina Milheiro</t>
+        </is>
+      </c>
+      <c r="C46" t="inlineStr">
+        <is>
+          <t>Catarina Milheiro</t>
+        </is>
+      </c>
+      <c r="D46" t="inlineStr">
+        <is>
+          <t>Catarina Milheiro</t>
+        </is>
+      </c>
+      <c r="E46" t="n">
+        <v>6</v>
+      </c>
+      <c r="F46" t="n">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="47">
+      <c r="A47" t="inlineStr">
+        <is>
+          <t>Catarina Milheiro</t>
+        </is>
+      </c>
+      <c r="B47" t="inlineStr">
+        <is>
+          <t>Catarina Milheiro</t>
+        </is>
+      </c>
+      <c r="C47" t="inlineStr">
+        <is>
+          <t>Catarina Milheiro</t>
+        </is>
+      </c>
+      <c r="E47" t="n">
+        <v>6</v>
+      </c>
+      <c r="F47" t="n">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="48">
+      <c r="B48" t="inlineStr">
+        <is>
+          <t>Catarina Milheiro</t>
+        </is>
+      </c>
+      <c r="E48" t="n">
+        <v>4</v>
+      </c>
+      <c r="F48" t="n">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="49">
+      <c r="A49" t="inlineStr">
+        <is>
+          <t>Catarina Milheiro</t>
+        </is>
+      </c>
+      <c r="B49" t="inlineStr">
+        <is>
+          <t>Catarina Milheiro</t>
+        </is>
+      </c>
+      <c r="C49" t="inlineStr">
+        <is>
+          <t>Gonçalo Figueiredo</t>
+        </is>
+      </c>
+      <c r="D49" t="inlineStr">
+        <is>
+          <t>Gonçalo Figueiredo</t>
+        </is>
+      </c>
+      <c r="E49" t="n">
+        <v>4</v>
+      </c>
+      <c r="F49" t="n">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="50">
+      <c r="B50" t="inlineStr">
+        <is>
+          <t>Catarina Milheiro</t>
+        </is>
+      </c>
+      <c r="C50" t="inlineStr">
+        <is>
+          <t>Inês Cabral</t>
+        </is>
+      </c>
+      <c r="D50" t="inlineStr">
+        <is>
+          <t>Inês Cabral</t>
+        </is>
+      </c>
+      <c r="E50" t="n">
+        <v>4</v>
+      </c>
+      <c r="F50" t="n">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="51">
+      <c r="A51" t="inlineStr">
+        <is>
+          <t>Catarina Milheiro</t>
+        </is>
+      </c>
+      <c r="B51" t="inlineStr">
+        <is>
+          <t>Catarina Milheiro</t>
+        </is>
+      </c>
+      <c r="C51" t="inlineStr">
+        <is>
+          <t>Inês Cabral</t>
+        </is>
+      </c>
+      <c r="E51" t="n">
+        <v>4</v>
+      </c>
+      <c r="F51" t="n">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="52">
+      <c r="B52" t="inlineStr">
+        <is>
           <t>Inês Bastos</t>
         </is>
       </c>
-      <c r="B29" t="inlineStr">
+      <c r="E52" t="n">
+        <v>6</v>
+      </c>
+      <c r="F52" t="n">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="53">
+      <c r="A53" t="inlineStr">
         <is>
           <t>Inês Bastos</t>
         </is>
       </c>
-      <c r="C29" t="inlineStr">
-        <is>
-          <t>Gonçalo Figueiredo</t>
-        </is>
-      </c>
-      <c r="D29" t="inlineStr">
-        <is>
-          <t>Gonçalo Figueiredo</t>
-        </is>
-      </c>
-      <c r="E29" t="n">
-        <v>4</v>
-      </c>
-      <c r="F29" t="n">
+      <c r="B53" t="inlineStr">
+        <is>
+          <t>Inês Bastos</t>
+        </is>
+      </c>
+      <c r="C53" t="inlineStr">
+        <is>
+          <t>Catarina Milheiro</t>
+        </is>
+      </c>
+      <c r="D53" t="inlineStr">
+        <is>
+          <t>Catarina Milheiro</t>
+        </is>
+      </c>
+      <c r="E53" t="n">
+        <v>6</v>
+      </c>
+      <c r="F53" t="n">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="54">
+      <c r="B54" t="inlineStr">
+        <is>
+          <t>Inês Bastos</t>
+        </is>
+      </c>
+      <c r="C54" t="inlineStr">
+        <is>
+          <t>Gonçalo Figueiredo</t>
+        </is>
+      </c>
+      <c r="D54" t="inlineStr">
+        <is>
+          <t>Gonçalo Figueiredo</t>
+        </is>
+      </c>
+      <c r="E54" t="n">
+        <v>4</v>
+      </c>
+      <c r="F54" t="n">
         <v>3</v>
       </c>
     </row>
-    <row r="30">
-      <c r="A30" t="inlineStr">
+    <row r="55">
+      <c r="A55" t="inlineStr">
         <is>
           <t>Inês Bastos</t>
         </is>
       </c>
-      <c r="B30" t="inlineStr">
+      <c r="B55" t="inlineStr">
         <is>
           <t>Inês Bastos</t>
         </is>
       </c>
-      <c r="D30" t="inlineStr">
-        <is>
-          <t>Inês Cabral</t>
-        </is>
-      </c>
-      <c r="E30" t="n">
-        <v>4</v>
-      </c>
-      <c r="F30" t="n">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="31"/>
-    <row r="32"/>
-    <row r="33"/>
-    <row r="34"/>
-    <row r="35"/>
-    <row r="36"/>
-    <row r="37"/>
-    <row r="38"/>
-    <row r="39"/>
-    <row r="40"/>
-    <row r="41"/>
-    <row r="42"/>
-    <row r="43"/>
-    <row r="44"/>
-    <row r="45"/>
-    <row r="46"/>
-    <row r="47"/>
-    <row r="48"/>
-    <row r="49"/>
-    <row r="50"/>
-    <row r="51"/>
-    <row r="52"/>
-    <row r="53"/>
-    <row r="54"/>
-    <row r="55"/>
-    <row r="56"/>
-    <row r="57"/>
+      <c r="D55" t="inlineStr">
+        <is>
+          <t>Gonçalo Figueiredo</t>
+        </is>
+      </c>
+      <c r="E55" t="n">
+        <v>4</v>
+      </c>
+      <c r="F55" t="n">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="56">
+      <c r="D56" t="inlineStr">
+        <is>
+          <t>Inês Cabral</t>
+        </is>
+      </c>
+      <c r="E56" t="n">
+        <v>4</v>
+      </c>
+      <c r="F56" t="n">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="57">
+      <c r="A57" t="inlineStr">
+        <is>
+          <t>Inês Bastos</t>
+        </is>
+      </c>
+      <c r="D57" t="inlineStr">
+        <is>
+          <t>Inês Cabral</t>
+        </is>
+      </c>
+      <c r="E57" t="n">
+        <v>4</v>
+      </c>
+      <c r="F57" t="n">
+        <v>4</v>
+      </c>
+    </row>
     <row r="58"/>
     <row r="59"/>
     <row r="60"/>
@@ -1195,121 +1654,168 @@
     <row r="85"/>
     <row r="86"/>
     <row r="87"/>
+    <row r="88"/>
+    <row r="89"/>
+    <row r="90"/>
+    <row r="91"/>
+    <row r="92"/>
+    <row r="93"/>
+    <row r="94"/>
+    <row r="95"/>
+    <row r="96"/>
+    <row r="97"/>
+    <row r="98"/>
+    <row r="99"/>
+    <row r="100"/>
+    <row r="101"/>
+    <row r="102"/>
+    <row r="103"/>
+    <row r="104"/>
+    <row r="105"/>
+    <row r="106"/>
+    <row r="107"/>
+    <row r="108"/>
+    <row r="109"/>
+    <row r="110"/>
+    <row r="111"/>
+    <row r="112"/>
+    <row r="113"/>
+    <row r="114"/>
+    <row r="115"/>
+    <row r="116"/>
+    <row r="117"/>
+    <row r="118"/>
+    <row r="119"/>
+    <row r="120"/>
+    <row r="121"/>
+    <row r="122"/>
+    <row r="123"/>
+    <row r="124"/>
+    <row r="125"/>
+    <row r="126"/>
+    <row r="127"/>
+    <row r="128"/>
+    <row r="129"/>
+    <row r="130"/>
+    <row r="131"/>
+    <row r="132"/>
+    <row r="133"/>
+    <row r="134"/>
+    <row r="135"/>
+    <row r="136"/>
+    <row r="137"/>
+    <row r="138"/>
+    <row r="139"/>
+    <row r="140"/>
+    <row r="141"/>
+    <row r="142"/>
+    <row r="143"/>
+    <row r="144"/>
+    <row r="145"/>
+    <row r="146"/>
+    <row r="147"/>
+    <row r="148"/>
+    <row r="149"/>
+    <row r="150"/>
+    <row r="151"/>
+    <row r="152"/>
   </sheetData>
-  <mergeCells count="113">
-    <mergeCell ref="B22:C22"/>
-    <mergeCell ref="B31:C31"/>
-    <mergeCell ref="A70:B70"/>
-    <mergeCell ref="B12:C12"/>
-    <mergeCell ref="B21:C21"/>
-    <mergeCell ref="A7:B7"/>
-    <mergeCell ref="A77"/>
-    <mergeCell ref="A83"/>
-    <mergeCell ref="B67:C67"/>
-    <mergeCell ref="B13:C13"/>
-    <mergeCell ref="B69:C69"/>
-    <mergeCell ref="B78:C78"/>
-    <mergeCell ref="A69"/>
-    <mergeCell ref="B40:C40"/>
-    <mergeCell ref="A84"/>
-    <mergeCell ref="A66"/>
-    <mergeCell ref="B49:C49"/>
-    <mergeCell ref="A75"/>
-    <mergeCell ref="B55:C55"/>
-    <mergeCell ref="B24:C24"/>
-    <mergeCell ref="B64:C64"/>
-    <mergeCell ref="A50"/>
-    <mergeCell ref="B33:C33"/>
-    <mergeCell ref="B51:C51"/>
-    <mergeCell ref="A86"/>
-    <mergeCell ref="B63:C63"/>
-    <mergeCell ref="A32"/>
-    <mergeCell ref="A29"/>
-    <mergeCell ref="A81"/>
-    <mergeCell ref="A38"/>
-    <mergeCell ref="B66:C66"/>
-    <mergeCell ref="B18:C18"/>
-    <mergeCell ref="B27:C27"/>
-    <mergeCell ref="A79:B79"/>
-    <mergeCell ref="A44"/>
-    <mergeCell ref="A61:B61"/>
-    <mergeCell ref="A15"/>
-    <mergeCell ref="A24"/>
-    <mergeCell ref="A51"/>
-    <mergeCell ref="A60"/>
-    <mergeCell ref="B37:C37"/>
-    <mergeCell ref="B84:C84"/>
-    <mergeCell ref="A27"/>
-    <mergeCell ref="B6:C6"/>
-    <mergeCell ref="A52:B52"/>
-    <mergeCell ref="B15:C15"/>
-    <mergeCell ref="A18"/>
-    <mergeCell ref="A42"/>
-    <mergeCell ref="A47"/>
-    <mergeCell ref="A34:B34"/>
-    <mergeCell ref="B54:C54"/>
-    <mergeCell ref="A35"/>
-    <mergeCell ref="A2:B3"/>
-    <mergeCell ref="A62"/>
-    <mergeCell ref="B72:C72"/>
-    <mergeCell ref="B81:C81"/>
-    <mergeCell ref="A20"/>
-    <mergeCell ref="A72"/>
-    <mergeCell ref="A6:A7"/>
-    <mergeCell ref="B58:C58"/>
-    <mergeCell ref="A48"/>
-    <mergeCell ref="A30"/>
-    <mergeCell ref="A59"/>
-    <mergeCell ref="B42:C42"/>
-    <mergeCell ref="B60:C60"/>
-    <mergeCell ref="B57:C57"/>
-    <mergeCell ref="B82:C82"/>
-    <mergeCell ref="A4:A5"/>
-    <mergeCell ref="B19:C19"/>
-    <mergeCell ref="B28:C28"/>
-    <mergeCell ref="A54"/>
-    <mergeCell ref="B9:C9"/>
-    <mergeCell ref="A41"/>
-    <mergeCell ref="B30:C30"/>
-    <mergeCell ref="A74"/>
-    <mergeCell ref="A56"/>
-    <mergeCell ref="A26"/>
-    <mergeCell ref="A43:B43"/>
-    <mergeCell ref="G1:H1"/>
+  <mergeCells count="95">
+    <mergeCell ref="C47:D48"/>
+    <mergeCell ref="A139:B140"/>
+    <mergeCell ref="C31:D32"/>
+    <mergeCell ref="A51:A52"/>
+    <mergeCell ref="A7:A8"/>
+    <mergeCell ref="C51:D52"/>
+    <mergeCell ref="C95:D96"/>
+    <mergeCell ref="A71:A72"/>
+    <mergeCell ref="C131:D132"/>
+    <mergeCell ref="A99:A100"/>
+    <mergeCell ref="A113:A114"/>
+    <mergeCell ref="A85:A86"/>
+    <mergeCell ref="A151:A152"/>
+    <mergeCell ref="A43:B44"/>
+    <mergeCell ref="B55:C58"/>
+    <mergeCell ref="A141:A142"/>
+    <mergeCell ref="A33:A34"/>
+    <mergeCell ref="A107:B108"/>
+    <mergeCell ref="A125:A126"/>
+    <mergeCell ref="A77:A78"/>
+    <mergeCell ref="A143:A144"/>
+    <mergeCell ref="A53:A54"/>
+    <mergeCell ref="A35:A36"/>
+    <mergeCell ref="A127:A128"/>
+    <mergeCell ref="C143:D144"/>
+    <mergeCell ref="A117:A118"/>
+    <mergeCell ref="C35:D36"/>
+    <mergeCell ref="B71:C74"/>
+    <mergeCell ref="A75:B76"/>
+    <mergeCell ref="A111:A112"/>
+    <mergeCell ref="B23:C26"/>
+    <mergeCell ref="C115:D116"/>
+    <mergeCell ref="C127:D128"/>
+    <mergeCell ref="A3:B4"/>
+    <mergeCell ref="A79:A80"/>
+    <mergeCell ref="C99:D100"/>
+    <mergeCell ref="A61:A62"/>
+    <mergeCell ref="A119:A120"/>
+    <mergeCell ref="A45:A46"/>
+    <mergeCell ref="A103:A104"/>
+    <mergeCell ref="C67:D68"/>
+    <mergeCell ref="A87:A88"/>
+    <mergeCell ref="A65:A66"/>
+    <mergeCell ref="A145:A146"/>
+    <mergeCell ref="G1:H2"/>
+    <mergeCell ref="A37:A38"/>
+    <mergeCell ref="A129:A130"/>
+    <mergeCell ref="A147:A148"/>
+    <mergeCell ref="A21:A22"/>
+    <mergeCell ref="A17:A18"/>
+    <mergeCell ref="A131:A132"/>
+    <mergeCell ref="A23:A24"/>
+    <mergeCell ref="A123:B124"/>
+    <mergeCell ref="A63:A64"/>
+    <mergeCell ref="A115:A116"/>
+    <mergeCell ref="A19:A20"/>
+    <mergeCell ref="A39:A40"/>
+    <mergeCell ref="A49:A50"/>
+    <mergeCell ref="A149:A150"/>
+    <mergeCell ref="B119:C122"/>
+    <mergeCell ref="C111:D112"/>
+    <mergeCell ref="A13:A14"/>
+    <mergeCell ref="C15:D16"/>
+    <mergeCell ref="C147:D148"/>
+    <mergeCell ref="A97:A98"/>
+    <mergeCell ref="C79:D80"/>
+    <mergeCell ref="A93:A94"/>
     <mergeCell ref="A1:F1"/>
-    <mergeCell ref="B76:C76"/>
-    <mergeCell ref="B45:C45"/>
-    <mergeCell ref="B85:C85"/>
-    <mergeCell ref="A71"/>
-    <mergeCell ref="A33"/>
-    <mergeCell ref="B75:C75"/>
-    <mergeCell ref="A8"/>
-    <mergeCell ref="A17"/>
-    <mergeCell ref="A53"/>
-    <mergeCell ref="B46:C46"/>
-    <mergeCell ref="A63"/>
-    <mergeCell ref="A68"/>
-    <mergeCell ref="B39:C39"/>
-    <mergeCell ref="A16:B16"/>
-    <mergeCell ref="B48:C48"/>
-    <mergeCell ref="A9"/>
-    <mergeCell ref="A25:B25"/>
-    <mergeCell ref="A39"/>
-    <mergeCell ref="A36"/>
-    <mergeCell ref="A11"/>
-    <mergeCell ref="A45"/>
-    <mergeCell ref="B73:C73"/>
-    <mergeCell ref="A78"/>
-    <mergeCell ref="A87"/>
-    <mergeCell ref="B10:C10"/>
-    <mergeCell ref="A65"/>
-    <mergeCell ref="A80"/>
-    <mergeCell ref="A12"/>
-    <mergeCell ref="A21"/>
-    <mergeCell ref="A57"/>
-    <mergeCell ref="B36:C36"/>
-    <mergeCell ref="A14"/>
-    <mergeCell ref="A23"/>
+    <mergeCell ref="C63:D64"/>
+    <mergeCell ref="A83:A84"/>
+    <mergeCell ref="A31:A32"/>
+    <mergeCell ref="A67:A68"/>
+    <mergeCell ref="A27:B28"/>
+    <mergeCell ref="B39:C42"/>
+    <mergeCell ref="A91:B92"/>
+    <mergeCell ref="A69:A70"/>
+    <mergeCell ref="B103:C106"/>
+    <mergeCell ref="A133:A134"/>
+    <mergeCell ref="B87:C90"/>
+    <mergeCell ref="A55:A56"/>
+    <mergeCell ref="C19:D20"/>
+    <mergeCell ref="A95:A96"/>
+    <mergeCell ref="A135:A136"/>
+    <mergeCell ref="A101:A102"/>
+    <mergeCell ref="A5:A6"/>
+    <mergeCell ref="B135:C138"/>
+    <mergeCell ref="C83:D84"/>
+    <mergeCell ref="A59:B60"/>
+    <mergeCell ref="A109:A110"/>
+    <mergeCell ref="B7:C10"/>
+    <mergeCell ref="A11:B12"/>
+    <mergeCell ref="A29:A30"/>
+    <mergeCell ref="A47:A48"/>
+    <mergeCell ref="A81:A82"/>
+    <mergeCell ref="A15:A16"/>
   </mergeCells>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
depois de 500 anos, isto voltou a funcionar e o codigo já está mais organizado, agora vou me focar nas opções de estilo
</commit_message>
<xml_diff>
--- a/output/Output-Avaliacao-Membro-RH.xlsx
+++ b/output/Output-Avaliacao-Membro-RH.xlsx
@@ -483,14 +483,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="7">
-      <c r="E7" t="n">
-        <v>5</v>
-      </c>
-      <c r="F7" t="n">
-        <v>5</v>
-      </c>
-    </row>
+    <row r="7"/>
     <row r="8">
       <c r="C8" t="inlineStr">
         <is>
@@ -504,14 +497,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="9">
-      <c r="E9" t="n">
-        <v>5</v>
-      </c>
-      <c r="F9" t="n">
-        <v>5</v>
-      </c>
-    </row>
+    <row r="9"/>
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
@@ -544,14 +530,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="13">
-      <c r="E13" t="n">
-        <v>4</v>
-      </c>
-      <c r="F13" t="n">
-        <v>5</v>
-      </c>
-    </row>
+    <row r="13"/>
     <row r="14">
       <c r="C14" t="inlineStr">
         <is>
@@ -565,14 +544,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="15">
-      <c r="E15" t="n">
-        <v>4</v>
-      </c>
-      <c r="F15" t="n">
-        <v>5</v>
-      </c>
-    </row>
+    <row r="15"/>
     <row r="16">
       <c r="A16" t="inlineStr">
         <is>
@@ -605,14 +577,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="19">
-      <c r="E19" t="n">
-        <v>3</v>
-      </c>
-      <c r="F19" t="n">
-        <v>2</v>
-      </c>
-    </row>
+    <row r="19"/>
     <row r="20">
       <c r="C20" t="inlineStr">
         <is>
@@ -626,14 +591,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="21">
-      <c r="E21" t="n">
-        <v>5</v>
-      </c>
-      <c r="F21" t="n">
-        <v>5</v>
-      </c>
-    </row>
+    <row r="21"/>
     <row r="22">
       <c r="A22" t="inlineStr">
         <is>
@@ -666,14 +624,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="25">
-      <c r="E25" t="n">
-        <v>6</v>
-      </c>
-      <c r="F25" t="n">
-        <v>4</v>
-      </c>
-    </row>
+    <row r="25"/>
     <row r="26">
       <c r="C26" t="inlineStr">
         <is>
@@ -687,14 +638,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="27">
-      <c r="E27" t="n">
-        <v>6</v>
-      </c>
-      <c r="F27" t="n">
-        <v>5</v>
-      </c>
-    </row>
+    <row r="27"/>
     <row r="28">
       <c r="A28" t="inlineStr">
         <is>
@@ -727,14 +671,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="31">
-      <c r="E31" t="n">
-        <v>5</v>
-      </c>
-      <c r="F31" t="n">
-        <v>5</v>
-      </c>
-    </row>
+    <row r="31"/>
     <row r="32">
       <c r="C32" t="inlineStr">
         <is>
@@ -748,14 +685,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="33">
-      <c r="E33" t="n">
-        <v>6</v>
-      </c>
-      <c r="F33" t="n">
-        <v>5</v>
-      </c>
-    </row>
+    <row r="33"/>
     <row r="34">
       <c r="A34" t="inlineStr">
         <is>
@@ -788,14 +718,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="37">
-      <c r="E37" t="n">
-        <v>5</v>
-      </c>
-      <c r="F37" t="n">
-        <v>4</v>
-      </c>
-    </row>
+    <row r="37"/>
     <row r="38">
       <c r="C38" t="inlineStr">
         <is>
@@ -809,14 +732,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="39">
-      <c r="E39" t="n">
-        <v>5</v>
-      </c>
-      <c r="F39" t="n">
-        <v>4</v>
-      </c>
-    </row>
+    <row r="39"/>
     <row r="40">
       <c r="A40" t="inlineStr">
         <is>
@@ -849,14 +765,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="43">
-      <c r="E43" t="n">
-        <v>4</v>
-      </c>
-      <c r="F43" t="n">
-        <v>4</v>
-      </c>
-    </row>
+    <row r="43"/>
     <row r="44">
       <c r="C44" t="inlineStr">
         <is>
@@ -870,14 +779,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="45">
-      <c r="E45" t="n">
-        <v>6</v>
-      </c>
-      <c r="F45" t="n">
-        <v>6</v>
-      </c>
-    </row>
+    <row r="45"/>
     <row r="46">
       <c r="A46" t="inlineStr">
         <is>
@@ -910,14 +812,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="49">
-      <c r="E49" t="n">
-        <v>4</v>
-      </c>
-      <c r="F49" t="n">
-        <v>4</v>
-      </c>
-    </row>
+    <row r="49"/>
     <row r="50">
       <c r="C50" t="inlineStr">
         <is>
@@ -931,14 +826,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="51">
-      <c r="E51" t="n">
-        <v>4</v>
-      </c>
-      <c r="F51" t="n">
-        <v>4</v>
-      </c>
-    </row>
+    <row r="51"/>
     <row r="52">
       <c r="A52" t="inlineStr">
         <is>
@@ -971,14 +859,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="55">
-      <c r="E55" t="n">
-        <v>4</v>
-      </c>
-      <c r="F55" t="n">
-        <v>3</v>
-      </c>
-    </row>
+    <row r="55"/>
     <row r="56">
       <c r="C56" t="inlineStr">
         <is>
@@ -992,75 +873,104 @@
         <v>4</v>
       </c>
     </row>
-    <row r="57">
-      <c r="E57" t="n">
-        <v>4</v>
-      </c>
-      <c r="F57" t="n">
-        <v>4</v>
-      </c>
-    </row>
+    <row r="57"/>
   </sheetData>
-  <mergeCells count="59">
+  <mergeCells count="95">
+    <mergeCell ref="F44:F45"/>
+    <mergeCell ref="E8:E9"/>
+    <mergeCell ref="E48:E49"/>
+    <mergeCell ref="E10:E11"/>
+    <mergeCell ref="F18:F19"/>
+    <mergeCell ref="C8:D9"/>
+    <mergeCell ref="F30:F31"/>
+    <mergeCell ref="F26:F27"/>
+    <mergeCell ref="C48:D49"/>
+    <mergeCell ref="F42:F43"/>
+    <mergeCell ref="C38:D39"/>
+    <mergeCell ref="E2:E3"/>
+    <mergeCell ref="A4:B9"/>
+    <mergeCell ref="C34:D35"/>
+    <mergeCell ref="F28:F29"/>
+    <mergeCell ref="A40:B45"/>
+    <mergeCell ref="E50:E51"/>
+    <mergeCell ref="F48:F49"/>
+    <mergeCell ref="C42:D43"/>
+    <mergeCell ref="C20:D21"/>
+    <mergeCell ref="E12:E13"/>
+    <mergeCell ref="C50:D51"/>
+    <mergeCell ref="C44:D45"/>
+    <mergeCell ref="F34:F35"/>
+    <mergeCell ref="C22:D23"/>
+    <mergeCell ref="F16:F17"/>
+    <mergeCell ref="E14:E15"/>
     <mergeCell ref="F40:F41"/>
     <mergeCell ref="A16:B21"/>
     <mergeCell ref="C12:D13"/>
-    <mergeCell ref="A2:B3"/>
-    <mergeCell ref="C46:D47"/>
-    <mergeCell ref="C2:D3"/>
-    <mergeCell ref="C40:D41"/>
     <mergeCell ref="E4:E5"/>
+    <mergeCell ref="F36:F37"/>
     <mergeCell ref="C36:D37"/>
-    <mergeCell ref="F16:F17"/>
-    <mergeCell ref="E34:E35"/>
-    <mergeCell ref="C52:D53"/>
-    <mergeCell ref="E10:E11"/>
+    <mergeCell ref="F20:F21"/>
     <mergeCell ref="F2:F3"/>
-    <mergeCell ref="C8:D9"/>
-    <mergeCell ref="A46:B51"/>
-    <mergeCell ref="C32:D33"/>
+    <mergeCell ref="E38:E39"/>
     <mergeCell ref="F22:F23"/>
-    <mergeCell ref="E28:E29"/>
-    <mergeCell ref="F34:F35"/>
-    <mergeCell ref="C48:D49"/>
     <mergeCell ref="E46:E47"/>
-    <mergeCell ref="C38:D39"/>
-    <mergeCell ref="E2:E3"/>
-    <mergeCell ref="A22:B27"/>
     <mergeCell ref="E40:E41"/>
-    <mergeCell ref="A4:B9"/>
-    <mergeCell ref="C34:D35"/>
-    <mergeCell ref="C28:D29"/>
-    <mergeCell ref="C6:D7"/>
+    <mergeCell ref="E54:E55"/>
     <mergeCell ref="C24:D25"/>
-    <mergeCell ref="C18:D19"/>
-    <mergeCell ref="A34:B39"/>
-    <mergeCell ref="A10:B15"/>
-    <mergeCell ref="A28:B33"/>
-    <mergeCell ref="F28:F29"/>
-    <mergeCell ref="F52:F53"/>
     <mergeCell ref="F46:F47"/>
-    <mergeCell ref="C14:D15"/>
-    <mergeCell ref="A40:B45"/>
-    <mergeCell ref="E16:E17"/>
-    <mergeCell ref="C30:D31"/>
-    <mergeCell ref="A52:B57"/>
-    <mergeCell ref="C4:D5"/>
-    <mergeCell ref="C42:D43"/>
-    <mergeCell ref="C20:D21"/>
+    <mergeCell ref="E26:E27"/>
     <mergeCell ref="C10:D11"/>
     <mergeCell ref="C16:D17"/>
     <mergeCell ref="F4:F5"/>
+    <mergeCell ref="C26:D27"/>
+    <mergeCell ref="F10:F11"/>
+    <mergeCell ref="F54:F55"/>
+    <mergeCell ref="F24:F25"/>
+    <mergeCell ref="E52:E53"/>
+    <mergeCell ref="A2:B3"/>
+    <mergeCell ref="C2:D3"/>
+    <mergeCell ref="E42:E43"/>
+    <mergeCell ref="E20:E21"/>
+    <mergeCell ref="C52:D53"/>
+    <mergeCell ref="E44:E45"/>
+    <mergeCell ref="A46:B51"/>
+    <mergeCell ref="F8:F9"/>
+    <mergeCell ref="E28:E29"/>
+    <mergeCell ref="F50:F51"/>
+    <mergeCell ref="A22:B27"/>
+    <mergeCell ref="E30:E31"/>
+    <mergeCell ref="C28:D29"/>
+    <mergeCell ref="E32:E33"/>
+    <mergeCell ref="C6:D7"/>
+    <mergeCell ref="A34:B39"/>
+    <mergeCell ref="F52:F53"/>
+    <mergeCell ref="A28:B33"/>
+    <mergeCell ref="E16:E17"/>
+    <mergeCell ref="C30:D31"/>
+    <mergeCell ref="F14:F15"/>
+    <mergeCell ref="E56:E57"/>
+    <mergeCell ref="C54:D55"/>
+    <mergeCell ref="E18:E19"/>
     <mergeCell ref="A1:F1"/>
-    <mergeCell ref="C54:D55"/>
+    <mergeCell ref="F6:F7"/>
+    <mergeCell ref="C56:D57"/>
+    <mergeCell ref="C46:D47"/>
+    <mergeCell ref="C40:D41"/>
+    <mergeCell ref="F12:F13"/>
+    <mergeCell ref="E34:E35"/>
+    <mergeCell ref="F32:F33"/>
+    <mergeCell ref="C32:D33"/>
+    <mergeCell ref="F56:F57"/>
+    <mergeCell ref="E6:E7"/>
+    <mergeCell ref="F38:F39"/>
+    <mergeCell ref="C18:D19"/>
+    <mergeCell ref="A10:B15"/>
+    <mergeCell ref="E36:E37"/>
+    <mergeCell ref="C14:D15"/>
+    <mergeCell ref="A52:B57"/>
+    <mergeCell ref="C4:D5"/>
     <mergeCell ref="E22:E23"/>
-    <mergeCell ref="C50:D51"/>
-    <mergeCell ref="C26:D27"/>
-    <mergeCell ref="C44:D45"/>
-    <mergeCell ref="C22:D23"/>
-    <mergeCell ref="F10:F11"/>
-    <mergeCell ref="C56:D57"/>
-    <mergeCell ref="E52:E53"/>
+    <mergeCell ref="E24:E25"/>
   </mergeCells>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Corrigindo um bug com as cores das colunas
</commit_message>
<xml_diff>
--- a/output/Output-Avaliacao-Membro-RH.xlsx
+++ b/output/Output-Avaliacao-Membro-RH.xlsx
@@ -2,8 +2,9 @@
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
+  <workbookProtection/>
   <bookViews>
-    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
+    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId1"/>
@@ -132,7 +133,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" pivotButton="0" quotePrefix="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0" hidden="0"/>
   </cellStyles>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
   <colors>
@@ -497,7 +498,7 @@
   </sheetPr>
   <dimension ref="A1:X74"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
     </sheetView>
   </sheetViews>
@@ -641,7 +642,7 @@
           <t>5. O membro é capaz de executar a sua tarefa de forma eficaz e com qualidade, apresentando espírito crítico, ou seja, questionando e analisando-a de forma racional.</t>
         </is>
       </c>
-      <c r="X2" s="6" t="inlineStr">
+      <c r="X2" s="5" t="inlineStr">
         <is>
           <t>Observações</t>
         </is>
@@ -717,7 +718,7 @@
       <c r="W3" s="6" t="n">
         <v>6</v>
       </c>
-      <c r="X3" s="6" t="inlineStr">
+      <c r="X3" s="5" t="inlineStr">
         <is>
           <t>Em relação à minha avaliação: não tenho participado como queria no slack dando o feedback que os meus colegas merecem, mas é uma característica que estou a desenvolver agora que já me sinto mais habituada à dinâmica dos canais.</t>
         </is>
@@ -1262,7 +1263,7 @@
       <c r="W11" s="6" t="n">
         <v>6</v>
       </c>
-      <c r="X11" s="6" t="inlineStr">
+      <c r="X11" s="5" t="inlineStr">
         <is>
           <t>Em relação à minha avaliação: não tenho participado como queria no slack dando o feedback que os meus colegas merecem, mas é uma característica que estou a desenvolver agora que já me sinto mais habituada à dinâmica dos canais</t>
         </is>
@@ -1807,7 +1808,7 @@
       <c r="W19" s="6" t="n">
         <v>6</v>
       </c>
-      <c r="X19" s="6" t="inlineStr">
+      <c r="X19" s="5" t="inlineStr">
         <is>
           <t>Nada a apontar</t>
         </is>
@@ -2352,7 +2353,7 @@
       <c r="W27" s="6" t="n">
         <v>6</v>
       </c>
-      <c r="X27" s="6" t="inlineStr">
+      <c r="X27" s="5" t="inlineStr">
         <is>
           <t>Nada a apontar</t>
         </is>
@@ -2897,7 +2898,7 @@
       <c r="W35" s="6" t="n">
         <v>6</v>
       </c>
-      <c r="X35" s="6" t="inlineStr">
+      <c r="X35" s="5" t="inlineStr">
         <is>
           <t>Nada a apontar</t>
         </is>
@@ -3442,7 +3443,7 @@
       <c r="W43" s="6" t="n">
         <v>6</v>
       </c>
-      <c r="X43" s="6" t="inlineStr">
+      <c r="X43" s="5" t="inlineStr">
         <is>
           <t>Nada a apontar</t>
         </is>
@@ -3987,7 +3988,7 @@
       <c r="W51" s="6" t="n">
         <v>6</v>
       </c>
-      <c r="X51" s="6" t="inlineStr">
+      <c r="X51" s="5" t="inlineStr">
         <is>
           <t>Nada a apontar</t>
         </is>
@@ -4532,7 +4533,7 @@
       <c r="W59" s="6" t="n">
         <v>6</v>
       </c>
-      <c r="X59" s="6" t="inlineStr">
+      <c r="X59" s="5" t="inlineStr">
         <is>
           <t>Nada a apontar</t>
         </is>
@@ -5077,7 +5078,7 @@
       <c r="W67" s="6" t="n">
         <v>6</v>
       </c>
-      <c r="X67" s="6" t="inlineStr">
+      <c r="X67" s="5" t="inlineStr">
         <is>
           <t>Nada a apontar</t>
         </is>
@@ -7036,6 +7037,6 @@
     <mergeCell ref="C13:D13"/>
     <mergeCell ref="R42"/>
   </mergeCells>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
 </file>
</xml_diff>